<commit_message>
Cleanup and new Requirements added
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\VVS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DDFFA70-7201-42D9-BE02-DD2206CE9C29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A297D-2087-4EF1-8F4B-F779FE788A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="101">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -141,67 +141,10 @@
     <t>R02</t>
   </si>
   <si>
-    <t>R03</t>
-  </si>
-  <si>
     <t>R05</t>
   </si>
   <si>
     <t>The system shall provide a means to specify the recurance of one task also in days weeks and months, and that's because it's easier for user to intoduce 1 week recurance of an event than evaluat how many hour are in a week.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The system shall provide a method that shows the following task details:</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">	
-		- start date ( HH:mm dd:mm:yyyy or any other format) 
-		- end date ( HH:mm dd:mm:yyyy or any other format) 
-		- task status ( active/inactive )
-		- recurance status ( yes/no )
-		- recurance time-frame ( days, weeks, months )
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The system already have an interface with these information but the requirement was not explicit</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.</t>
-    </r>
   </si>
   <si>
     <t>The system shall provide a method to list all the task in a week based on the start day and week of that task (even and odd weeks).</t>
@@ -1505,12 +1448,66 @@
   <si>
     <t>Effort to perform tool-based code analysis (hours): 10 m</t>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The system shall provide a method that show the following task details:</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">	
+		- start date ( HH:mm dd:mm:yyyy or any other format) 
+		- end date ( HH:mm dd:mm:yyyy or any other format) 
+		- task status ( active/inactive )
+		- recurance status ( yes/no )
+		- recurance time-frame ( days, weeks, months )
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The system already have an interface with these information but the requirement was not explicit</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2092,24 +2089,24 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="47.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="70.140625" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="70.109375" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
     <col min="9" max="9" width="21" style="6" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="8.85546875" style="6"/>
+    <col min="10" max="10" width="14.44140625" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2120,7 +2117,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2135,7 +2132,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2146,7 +2143,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -2158,18 +2155,18 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
@@ -2182,7 +2179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -2192,7 +2189,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2201,7 +2198,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2215,7 +2212,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="45">
+    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2223,28 +2220,28 @@
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="120">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -2253,13 +2250,13 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="135">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2268,13 +2265,13 @@
         <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2283,28 +2280,28 @@
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="90">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2313,7 +2310,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2322,7 +2319,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2331,7 +2328,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2340,7 +2337,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2349,7 +2346,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2358,7 +2355,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2367,7 +2364,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2376,7 +2373,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2385,7 +2382,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2394,13 +2391,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -2424,22 +2421,22 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="78.7109375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="22.140625" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="16.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="78.6640625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="22.109375" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2450,7 +2447,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>15</v>
       </c>
@@ -2465,7 +2462,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2476,7 +2473,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -2488,13 +2485,13 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -2512,7 +2509,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -2522,7 +2519,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2531,7 +2528,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2545,58 +2542,58 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="75">
+    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="75">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="60">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="60">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2605,7 +2602,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2614,7 +2611,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2623,7 +2620,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2632,7 +2629,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2641,7 +2638,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2650,7 +2647,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2659,7 +2656,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2668,7 +2665,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2677,7 +2674,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2686,7 +2683,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2695,7 +2692,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2704,7 +2701,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2713,13 +2710,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2743,23 +2740,23 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="49.140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="67.7109375" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="49.109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="67.6640625" style="6" customWidth="1"/>
+    <col min="6" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2770,7 +2767,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>14</v>
       </c>
@@ -2785,7 +2782,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2796,7 +2793,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -2808,13 +2805,13 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2832,17 +2829,17 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2851,7 +2848,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2865,111 +2862,111 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30">
+    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="30">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="45">
+    </row>
+    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="1" t="s">
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="45">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="45">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="E14" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="30">
-      <c r="B15" s="3">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="30">
+    </row>
+    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2978,7 +2975,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2987,7 +2984,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2996,7 +2993,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3005,7 +3002,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3014,7 +3011,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3023,7 +3020,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3032,7 +3029,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3041,7 +3038,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3050,7 +3047,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3059,7 +3056,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3068,7 +3065,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3077,7 +3074,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3086,7 +3083,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3095,13 +3092,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -3125,24 +3122,24 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" style="6"/>
-    <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="55.85546875" style="6" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="79.5703125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="61.42578125" style="6" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="8.85546875" style="6"/>
+    <col min="1" max="1" width="8.88671875" style="6"/>
+    <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="55.88671875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="79.5546875" style="6" customWidth="1"/>
+    <col min="6" max="6" width="61.44140625" style="6" customWidth="1"/>
+    <col min="7" max="8" width="8.88671875" style="6"/>
+    <col min="9" max="9" width="26.6640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75">
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -3153,7 +3150,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B2" s="28" t="s">
         <v>28</v>
       </c>
@@ -3168,7 +3165,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -3179,25 +3176,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E4" s="35"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -3215,7 +3212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -3226,7 +3223,7 @@
       <c r="E6" s="26"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -3243,96 +3240,96 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="135">
+    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="105">
+    </row>
+    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="F13" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="45">
-      <c r="B13" s="3">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C13" s="1" t="s">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3342,7 +3339,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3352,7 +3349,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3362,7 +3359,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3372,7 +3369,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3382,7 +3379,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3392,7 +3389,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3402,7 +3399,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3412,7 +3409,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3422,7 +3419,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3432,7 +3429,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3442,7 +3439,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3452,7 +3449,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3462,7 +3459,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3472,7 +3469,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3482,7 +3479,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3492,15 +3489,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="38" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6">
+    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Validation layer and ignore some build files
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\VVS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE3A297D-2087-4EF1-8F4B-F779FE788A10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E278F660-242C-4D52-97F2-9656D2CD41A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -147,9 +147,6 @@
     <t>The system shall provide a means to specify the recurance of one task also in days weeks and months, and that's because it's easier for user to intoduce 1 week recurance of an event than evaluat how many hour are in a week.</t>
   </si>
   <si>
-    <t>The system shall provide a method to list all the task in a week based on the start day and week of that task (even and odd weeks).</t>
-  </si>
-  <si>
     <t>The system shall provide a means to display an error message to the user every time one of the followig forbidden actions is taken:
 		- filer task without having a start &amp; end date &amp; hour
 		- add a new task without:
@@ -1501,6 +1498,9 @@
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>The system shall provide a method to list all the task in a week based on the start day and start week of that task (even and odd weeks).</t>
   </si>
 </sst>
 </file>
@@ -2089,8 +2089,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,7 +2155,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
@@ -2166,7 +2166,7 @@
         <v>9</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="31"/>
       <c r="H5" s="17" t="s">
@@ -2220,7 +2220,7 @@
         <v>33</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>36</v>
@@ -2235,10 +2235,10 @@
         <v>33</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2250,10 +2250,10 @@
         <v>34</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
@@ -2265,10 +2265,10 @@
         <v>34</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2280,10 +2280,10 @@
         <v>34</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2295,10 +2295,10 @@
         <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2397,7 +2397,7 @@
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -2421,8 +2421,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2485,7 +2485,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
@@ -2547,11 +2547,11 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
@@ -2560,11 +2560,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2573,11 +2573,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2586,11 +2586,11 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -2716,7 +2716,7 @@
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -2805,7 +2805,7 @@
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
@@ -2835,7 +2835,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E6" s="26"/>
     </row>
@@ -2867,13 +2867,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2882,13 +2882,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2897,13 +2897,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2912,13 +2912,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -2927,13 +2927,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2942,13 +2942,13 @@
         <v>6</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2957,13 +2957,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
@@ -3098,7 +3098,7 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -3123,7 +3123,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3181,14 +3181,14 @@
         <v>22</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="35"/>
       <c r="H4" s="17" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="22" t="s">
         <v>31</v>
@@ -3245,16 +3245,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D10" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -3263,16 +3263,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="E11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
@@ -3281,16 +3281,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
@@ -3299,16 +3299,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -3317,16 +3317,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>95</v>
-      </c>
       <c r="E14" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -3491,7 +3491,7 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C32" s="38" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>

</xml_diff>

<commit_message>
Update excel for lab
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drago\Desktop\VVS\Docs\Lab01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E278F660-242C-4D52-97F2-9656D2CD41A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A99CC8-4AD9-4518-A2EA-F15C8088FD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -1318,11 +1318,6 @@
     </r>
   </si>
   <si>
-    <t>private TaskIO() {
-        throw new IllegalStateException("Utility class");
-    }</t>
-  </si>
-  <si>
     <t>The TaskIO class didn't have a private constructor</t>
   </si>
   <si>
@@ -1502,12 +1497,15 @@
   <si>
     <t>The system shall provide a method to list all the task in a week based on the start day and start week of that task (even and odd weeks).</t>
   </si>
+  <si>
+    <t>no action taken because all methods of that class are static.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2089,11 +2087,11 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -2106,7 +2104,7 @@
     <col min="11" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2117,7 +2115,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
@@ -2132,7 +2130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2143,7 +2141,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="13" t="s">
         <v>0</v>
       </c>
@@ -2161,7 +2159,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="13" t="s">
         <v>9</v>
       </c>
@@ -2179,7 +2177,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -2189,7 +2187,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2198,7 +2196,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2212,7 +2210,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="43.2">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2226,7 +2224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="115.2">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2238,10 +2236,10 @@
         <v>54</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="28.8">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B25" si="0">B11+1</f>
         <v>3</v>
@@ -2253,10 +2251,10 @@
         <v>53</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="129.6">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2271,7 +2269,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="28.8">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2286,7 +2284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="72">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2301,7 +2299,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2310,7 +2308,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2319,7 +2317,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2328,7 +2326,7 @@
       <c r="D18" s="3"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2337,7 +2335,7 @@
       <c r="D19" s="3"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2346,7 +2344,7 @@
       <c r="D20" s="3"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2355,7 +2353,7 @@
       <c r="D21" s="3"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2364,7 +2362,7 @@
       <c r="D22" s="3"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2373,7 +2371,7 @@
       <c r="D23" s="3"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2382,7 +2380,7 @@
       <c r="D24" s="3"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2391,13 +2389,13 @@
       <c r="D25" s="3"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="C27" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2421,11 +2419,11 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -2436,7 +2434,7 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2447,7 +2445,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2" s="28" t="s">
         <v>15</v>
       </c>
@@ -2462,7 +2460,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2473,7 +2471,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
@@ -2491,7 +2489,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
@@ -2509,7 +2507,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -2519,7 +2517,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2528,7 +2526,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2542,7 +2540,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="57.6">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2554,7 +2552,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="72">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2567,7 +2565,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="43.2">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
@@ -2580,7 +2578,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="43.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2593,7 +2591,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2602,7 +2600,7 @@
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2611,7 +2609,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2620,7 +2618,7 @@
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2629,7 +2627,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2638,7 +2636,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2647,7 +2645,7 @@
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -2656,7 +2654,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -2665,7 +2663,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -2674,7 +2672,7 @@
       <c r="D22" s="1"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -2683,7 +2681,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2692,7 +2690,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2701,7 +2699,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2710,13 +2708,13 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="C28" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2740,11 +2738,11 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -2756,7 +2754,7 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -2767,7 +2765,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2" s="28" t="s">
         <v>14</v>
       </c>
@@ -2782,7 +2780,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -2793,7 +2791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>0</v>
       </c>
@@ -2811,7 +2809,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="16" t="s">
         <v>9</v>
       </c>
@@ -2829,7 +2827,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
@@ -2839,7 +2837,7 @@
       </c>
       <c r="E6" s="26"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
@@ -2848,7 +2846,7 @@
       </c>
       <c r="E7" s="26"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -2862,7 +2860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="28.8">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -2876,7 +2874,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="28.8">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -2891,7 +2889,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="28.8">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -2906,7 +2904,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="43.2">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2921,7 +2919,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="43.2">
       <c r="B14" s="3">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2936,7 +2934,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="28.8">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -2951,7 +2949,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="28.8">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2966,7 +2964,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2975,7 +2973,7 @@
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2984,7 +2982,7 @@
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2993,7 +2991,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3002,7 +3000,7 @@
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3011,7 +3009,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3020,7 +3018,7 @@
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3029,7 +3027,7 @@
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3038,7 +3036,7 @@
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3047,7 +3045,7 @@
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3056,7 +3054,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3065,7 +3063,7 @@
       <c r="D27" s="2"/>
       <c r="E27" s="1"/>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3074,7 +3072,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3083,7 +3081,7 @@
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3092,13 +3090,13 @@
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5">
       <c r="C32" s="11" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -3122,11 +3120,11 @@
   </sheetPr>
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="6"/>
     <col min="2" max="2" width="12.33203125" style="6" customWidth="1"/>
@@ -3139,7 +3137,7 @@
     <col min="10" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="15.6">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>3</v>
@@ -3150,7 +3148,7 @@
       <c r="I1" s="27"/>
       <c r="J1" s="27"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="B2" s="28" t="s">
         <v>28</v>
       </c>
@@ -3165,7 +3163,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="H3" s="17" t="s">
         <v>17</v>
       </c>
@@ -3176,7 +3174,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="C4" s="16" t="s">
         <v>22</v>
       </c>
@@ -3194,7 +3192,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10">
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
@@ -3212,7 +3210,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>1</v>
@@ -3223,7 +3221,7 @@
       <c r="E6" s="26"/>
       <c r="F6" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10">
       <c r="B9" s="10" t="s">
         <v>4</v>
       </c>
@@ -3240,7 +3238,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="129.6">
       <c r="B10" s="3">
         <v>1</v>
       </c>
@@ -3257,7 +3255,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
@@ -3275,7 +3273,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="100.8">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B30" si="0">B11+1</f>
         <v>3</v>
@@ -3293,43 +3291,43 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="B14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="3">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:10">
       <c r="B15" s="3">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3339,7 +3337,7 @@
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10">
       <c r="B16" s="3">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3349,7 +3347,7 @@
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6">
       <c r="B17" s="3">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3359,7 +3357,7 @@
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6">
       <c r="B18" s="3">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -3369,7 +3367,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6">
       <c r="B19" s="3">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -3379,7 +3377,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6">
       <c r="B20" s="3">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -3389,7 +3387,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6">
       <c r="B21" s="3">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -3399,7 +3397,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6">
       <c r="B22" s="3">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -3409,7 +3407,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6">
       <c r="B23" s="3">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -3419,7 +3417,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6">
       <c r="B24" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -3429,7 +3427,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6">
       <c r="B25" s="3">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -3439,7 +3437,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6">
       <c r="B26" s="3">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -3449,7 +3447,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6">
       <c r="B27" s="3">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -3459,7 +3457,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6">
       <c r="B28" s="3">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -3469,7 +3467,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6">
       <c r="B29" s="3">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -3479,7 +3477,7 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6">
       <c r="B30" s="3">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -3489,15 +3487,15 @@
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6">
       <c r="C32" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D32" s="39"/>
       <c r="E32" s="39"/>
       <c r="F32" s="18"/>
     </row>
-    <row r="35" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:6">
       <c r="F35" s="21"/>
     </row>
   </sheetData>

</xml_diff>